<commit_message>
Modificacion de diseño y depuracion de temp
</commit_message>
<xml_diff>
--- a/dataprueba_table gouser.xlsx
+++ b/dataprueba_table gouser.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\ibrokergo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{66431653-D4F8-4C5E-B263-24155E340301}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDE61825-E65B-4CD8-AD52-5DF7AA6D10BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{2E389C4B-D693-4112-A905-A1329CCF5501}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="201">
   <si>
     <t>null</t>
   </si>
@@ -493,6 +494,147 @@
   </si>
   <si>
     <t>Reparo todo tipo de muebles o ventanas , ademas tambien realizo pintado y otras que tenga que ver con el rubro</t>
+  </si>
+  <si>
+    <t>INSERT INTO gouser VALUES ('null','2','David Cosio','150514','Av Santa Anita 234','13/05/2020 04:14','roy@gmail.com','$2y$10$Z34DID7EwF4QAxkzMDDjm.oeMZd1hYPRfvDMhTwnSNQ0HkH69CMH6','default','34568976','986846176','1','1','Reparo impresoras , laptops , escanner , instalación de programas informáticos , Instalación de Redes y cualquier articulo de oficina , espero les guste mi servicio , muchas gracias','4');</t>
+  </si>
+  <si>
+    <t>INSERT INTO gouser VALUES ('null','2','Abel Jesus  Bedoya  Zuñiga','150134','ANGAMOS OESTE NRO. 544 DPTO. 302 ','13/05/2020 04:14','intelect@intelect.com.pe','$2y$10$Z34DID7EwF4QAxkzMDDjm.oeMZd1hYPRfvDMhTwnSNQ0HkH69CMH6','default','14817982','998857023','1','1','Me dedico a la atencion de niños','3');</t>
+  </si>
+  <si>
+    <t>INSERT INTO gouser VALUES ('null','2','Abel Perez','150134','PASEO DE LA REPUBLICA NRO. 3195 INT. 503','13/05/2020 04:14','izapata@innovacion-empresarial.com','$2y$10$Z34DID7EwF4QAxkzMDDjm.oeMZd1hYPRfvDMhTwnSNQ0HkH69CMH6','default','22698694','997797705','1','1','Me llamo Anthony puente olano , me dedico a la fabricación de paredes , pintado y entre otras cosas','3');</t>
+  </si>
+  <si>
+    <t>INSERT INTO gouser VALUES ('null','2','Abel Ruiz Aguila','150134','LAS FRAGUAS NO.167','13/05/2020 04:14','consonniperu@consonniperu.com','$2y$10$Z34DID7EwF4QAxkzMDDjm.oeMZd1hYPRfvDMhTwnSNQ0HkH69CMH6','default','17316550','997249782','1','1','Reparo todo tipo de muebles o ventanas , ademas tambien realizo pintado y otras que tenga que ver con el rubro','2');</t>
+  </si>
+  <si>
+    <t>INSERT INTO gouser VALUES ('null','2','Abel Virgilio  Mattos  Jaque','150134','SAN JOSE NRO. 449 URB. SAN CARLOS','13/05/2020 04:14','ing_amattos@hotmail.com','$2y$10$Z34DID7EwF4QAxkzMDDjm.oeMZd1hYPRfvDMhTwnSNQ0HkH69CMH6','default','21514046','997394874','1','1','Reparo impresoras , laptops , escanner , instalación de programas informáticos , Instalación de Redes y cualquier articulo de oficina , espero les guste mi servicio , muchas gracias','8');</t>
+  </si>
+  <si>
+    <t>INSERT INTO gouser VALUES ('null','2','Abigail Mercedes  Morales  Corrales De Torres','150134','CAñON DEL PATO NRO. 103 (ESQ. CDRA. 5 AV. CAMINOS DEL INCA)','13/05/2020 04:14','tytl@tytl.com.pe','$2y$10$Z34DID7EwF4QAxkzMDDjm.oeMZd1hYPRfvDMhTwnSNQ0HkH69CMH6','default','14115613','996023789','1','1','Me dedico a la atencion de niños','8');</t>
+  </si>
+  <si>
+    <t>INSERT INTO gouser VALUES ('null','2','Abraham  Madrid  Ludeña','150134','JOSE MARTI NRO. 238 - MARANGA','13/05/2020 04:14','s3ggenerales@gmail.com','$2y$10$Z34DID7EwF4QAxkzMDDjm.oeMZd1hYPRfvDMhTwnSNQ0HkH69CMH6','default','12452500','993010449','1','1','Me llamo Anthony puente olano , me dedico a la fabricación de paredes , pintado y entre otras cosas','7');</t>
+  </si>
+  <si>
+    <t>INSERT INTO gouser VALUES ('null','2','Abraham Asuncion Vergara  Cordova','150134','PARURO NRO. 1207 ','13/05/2020 04:14','carlos_v2502@hotmail.com','$2y$10$Z34DID7EwF4QAxkzMDDjm.oeMZd1hYPRfvDMhTwnSNQ0HkH69CMH6','default','23130541','993539507','1','1','Reparo todo tipo de muebles o ventanas , ademas tambien realizo pintado y otras que tenga que ver con el rubro','4');</t>
+  </si>
+  <si>
+    <t>INSERT INTO gouser VALUES ('null','2','Abraham Douglas  Yorgest Urbina','150134','AZANGARO Nº 1024 OF. 15','13/05/2020 04:14','ayu_1@hotmail.com','$2y$10$Z34DID7EwF4QAxkzMDDjm.oeMZd1hYPRfvDMhTwnSNQ0HkH69CMH6','default','13066354','996138059','1','1','Reparo impresoras , laptops , escanner , instalación de programas informáticos , Instalación de Redes y cualquier articulo de oficina , espero les guste mi servicio , muchas gracias','5');</t>
+  </si>
+  <si>
+    <t>INSERT INTO gouser VALUES ('null','2','Ada Beatriz Cardoso Paredes','150134','JOSE NEYRA NRO. 244 INT. 201 URB. LA CALERA DE LA MERCED ','13/05/2020 04:14','a.cardoso@holistic-consultores.com','$2y$10$Z34DID7EwF4QAxkzMDDjm.oeMZd1hYPRfvDMhTwnSNQ0HkH69CMH6','default','20612528','992052487','1','1','Me dedico a la atencion de niños','2');</t>
+  </si>
+  <si>
+    <t>INSERT INTO gouser VALUES ('null','2','Ada Guillen  Castro','150134','CUSCO NRO. 417 INT. 704 ','13/05/2020 04:14','info@spavida.pe / rosof78@hotmail.com','$2y$10$Z34DID7EwF4QAxkzMDDjm.oeMZd1hYPRfvDMhTwnSNQ0HkH69CMH6','default','14811026','996213729','1','1','Me llamo Anthony puente olano , me dedico a la fabricación de paredes , pintado y entre otras cosas','5');</t>
+  </si>
+  <si>
+    <t>INSERT INTO gouser VALUES ('null','2','Ada Mori .','150137','JORGE BASADRE 1186 (POR LA EMBAJADA DE ESPAÑA)','13/05/2020 04:14','ncosta@floreztijero.com','$2y$10$Z34DID7EwF4QAxkzMDDjm.oeMZd1hYPRfvDMhTwnSNQ0HkH69CMH6','default','15224647','991507856','1','1','Reparo todo tipo de muebles o ventanas , ademas tambien realizo pintado y otras que tenga que ver con el rubro','9');</t>
+  </si>
+  <si>
+    <t>INSERT INTO gouser VALUES ('null','2','Ada Patricia  Camborda Montoya','150137','GRAL BORGOÑO NRO. 528 ','13/05/2020 04:14','estudio@abcmlegal.com','$2y$10$Z34DID7EwF4QAxkzMDDjm.oeMZd1hYPRfvDMhTwnSNQ0HkH69CMH6','default','12421604','991824258','1','1','Reparo impresoras , laptops , escanner , instalación de programas informáticos , Instalación de Redes y cualquier articulo de oficina , espero les guste mi servicio , muchas gracias','9');</t>
+  </si>
+  <si>
+    <t>INSERT INTO gouser VALUES ('null','2','Adalberto Eladio Carmona Gallo','150137','LAS HEBEAS NRO. 1284 URB. LOS JARDINES DE SAN JUAN','13/05/2020 04:14','adalcarmona@hotmail.com','$2y$10$Z34DID7EwF4QAxkzMDDjm.oeMZd1hYPRfvDMhTwnSNQ0HkH69CMH6','default','12773623','993700972','1','1','Me dedico a la atencion de niños','6');</t>
+  </si>
+  <si>
+    <t>INSERT INTO gouser VALUES ('null','2','Adalberto Seminario  Valle','150137','VIRREY TOLEDO NRO. 360 ','13/05/2020 04:14','jabelgui@gmail.com','$2y$10$Z34DID7EwF4QAxkzMDDjm.oeMZd1hYPRfvDMhTwnSNQ0HkH69CMH6','default','22260047','993150360','1','1','Me llamo Anthony puente olano , me dedico a la fabricación de paredes , pintado y entre otras cosas','1');</t>
+  </si>
+  <si>
+    <t>INSERT INTO gouser VALUES ('null','2','Adamo Gerolamo Angelo','150137','MARTIR OLAYA 129 OF. 1103','13/05/2020 04:14','j.vizcarra@aprilenet.com','$2y$10$Z34DID7EwF4QAxkzMDDjm.oeMZd1hYPRfvDMhTwnSNQ0HkH69CMH6','default','21980382','990967468','1','1','Reparo todo tipo de muebles o ventanas , ademas tambien realizo pintado y otras que tenga que ver con el rubro','5');</t>
+  </si>
+  <si>
+    <t>INSERT INTO gouser VALUES ('null','2','Adelina Astudillo G.','150137','STA. MARIA MAGDALENA NRO. 124','13/05/2020 04:14','kokenperu@amauta.rcp.net.pe','$2y$10$Z34DID7EwF4QAxkzMDDjm.oeMZd1hYPRfvDMhTwnSNQ0HkH69CMH6','default','23239192','992208412','1','1','Reparo impresoras , laptops , escanner , instalación de programas informáticos , Instalación de Redes y cualquier articulo de oficina , espero les guste mi servicio , muchas gracias','4');</t>
+  </si>
+  <si>
+    <t>INSERT INTO gouser VALUES ('null','2','Adolfo  Pinillos  Cordova','150137','PIO XII NRO. 480 INT. 301 URB. POLO HUNT ','13/05/2020 04:14','jjsantivanez@santivanezabogados.com','$2y$10$Z34DID7EwF4QAxkzMDDjm.oeMZd1hYPRfvDMhTwnSNQ0HkH69CMH6','default','13096292','999529514','1','1','Me dedico a la atencion de niños','1');</t>
+  </si>
+  <si>
+    <t>INSERT INTO gouser VALUES ('null','2','Adolfo Antonio  Chavez  Linares','150137','LOS LIBERTADORES NRO. 355 URB. SAN ISIDRO ','13/05/2020 04:14','contacto@achavezarquitectos.com','$2y$10$Z34DID7EwF4QAxkzMDDjm.oeMZd1hYPRfvDMhTwnSNQ0HkH69CMH6','default','14983813','998062638','1','1','Me llamo Anthony puente olano , me dedico a la fabricación de paredes , pintado y entre otras cosas','6');</t>
+  </si>
+  <si>
+    <t>INSERT INTO gouser VALUES ('null','2','Adolfo Auccapure .','150137','PUNKARI NRO. 1661 URB. MANGOMARCA ','13/05/2020 04:14','corpriseg@hotmail.com','$2y$10$Z34DID7EwF4QAxkzMDDjm.oeMZd1hYPRfvDMhTwnSNQ0HkH69CMH6','default','18626541','991894877','1','1','Reparo todo tipo de muebles o ventanas , ademas tambien realizo pintado y otras que tenga que ver con el rubro','4');</t>
+  </si>
+  <si>
+    <t>INSERT INTO gouser VALUES ('null','2','Adolfo Demetrio Mattos Rosel','150137','GERARDO UNGER NRO. 3273 ','13/05/2020 04:14','renviolmedios@renviol.com','$2y$10$Z34DID7EwF4QAxkzMDDjm.oeMZd1hYPRfvDMhTwnSNQ0HkH69CMH6','default','18474616','991120959','1','1','Reparo impresoras , laptops , escanner , instalación de programas informáticos , Instalación de Redes y cualquier articulo de oficina , espero les guste mi servicio , muchas gracias','7');</t>
+  </si>
+  <si>
+    <t>INSERT INTO gouser VALUES ('null','2','Adolfo Felix  Alvarez  Chauca','150137','ALCALÁ NRO. 492 DPTO. 301 URB. LA CASTELLANA ','13/05/2020 04:14','afac_g@yahoo.es','$2y$10$Z34DID7EwF4QAxkzMDDjm.oeMZd1hYPRfvDMhTwnSNQ0HkH69CMH6','default','13589139','999733276','1','1','Me dedico a la atencion de niños','7');</t>
+  </si>
+  <si>
+    <t>INSERT INTO gouser VALUES ('null','2','Adolfo Giorgio Draxl  Molina','150137','ALCALÁ NRO. 492 DPTO. 301 URB. LA CASTELLANA ','13/05/2020 04:14','info@gdbusiness.com.pe','$2y$10$Z34DID7EwF4QAxkzMDDjm.oeMZd1hYPRfvDMhTwnSNQ0HkH69CMH6','default','14418972','992512774','1','1','Me llamo Anthony puente olano , me dedico a la fabricación de paredes , pintado y entre otras cosas','3');</t>
+  </si>
+  <si>
+    <t>INSERT INTO gouser VALUES ('null','2','Adolfo Gygax Zegarra Ballon','150137','HAYA DE LA TORRE # 464(FTE.A LA ISLA DEL PARAISO)','13/05/2020 04:14','shurtado@orbislogistic.com','$2y$10$Z34DID7EwF4QAxkzMDDjm.oeMZd1hYPRfvDMhTwnSNQ0HkH69CMH6','default','21795089','996264916','1','1','Reparo todo tipo de muebles o ventanas , ademas tambien realizo pintado y otras que tenga que ver con el rubro','9');</t>
+  </si>
+  <si>
+    <t>INSERT INTO gouser VALUES ('null','2','Adolfo Mariscal Leal','150137','LAS AGUILAS  237','13/05/2020 04:14','amariscal@visual-presence.com','$2y$10$Z34DID7EwF4QAxkzMDDjm.oeMZd1hYPRfvDMhTwnSNQ0HkH69CMH6','default','20052337','994186266','1','1','Reparo impresoras , laptops , escanner , instalación de programas informáticos , Instalación de Redes y cualquier articulo de oficina , espero les guste mi servicio , muchas gracias','2');</t>
+  </si>
+  <si>
+    <t>INSERT INTO gouser VALUES ('null','2','Adolfo Valz-Gen Rivera','150137','ANGAMOS ESTE 2612 OF. 202','13/05/2020 04:14','adolfovalzgen@protezione.com.pe','$2y$10$Z34DID7EwF4QAxkzMDDjm.oeMZd1hYPRfvDMhTwnSNQ0HkH69CMH6','default','14029624','990777373','1','1','Me dedico a la atencion de niños','1');</t>
+  </si>
+  <si>
+    <t>INSERT INTO gouser VALUES ('null','2','Adolth Brown','150137','VICTOR ANDRES BELAUNDE #395','13/05/2020 04:14','oalvarado@ferrero.com.pe','$2y$10$Z34DID7EwF4QAxkzMDDjm.oeMZd1hYPRfvDMhTwnSNQ0HkH69CMH6','default','20861855','991953794','1','1','Me llamo Anthony puente olano , me dedico a la fabricación de paredes , pintado y entre otras cosas','8');</t>
+  </si>
+  <si>
+    <t>INSERT INTO gouser VALUES ('null','2','Adrian Poblete Espinosa','150103','AYACUCHO NRO. 328 INT. 328 URB. MIRAFLORES ','13/05/2020 04:14','clarosa@grupoincasac.com','$2y$10$Z34DID7EwF4QAxkzMDDjm.oeMZd1hYPRfvDMhTwnSNQ0HkH69CMH6','default','19442725','992304554','1','1','Reparo todo tipo de muebles o ventanas , ademas tambien realizo pintado y otras que tenga que ver con el rubro','5');</t>
+  </si>
+  <si>
+    <t>INSERT INTO gouser VALUES ('null','2','Adrian Revilla  Vergara','150103','SALAVERRY NRO. 3231','13/05/2020 04:14','abogados@reyrios.com','$2y$10$Z34DID7EwF4QAxkzMDDjm.oeMZd1hYPRfvDMhTwnSNQ0HkH69CMH6','default','23204344','993893103','1','1','Reparo impresoras , laptops , escanner , instalación de programas informáticos , Instalación de Redes y cualquier articulo de oficina , espero les guste mi servicio , muchas gracias','5');</t>
+  </si>
+  <si>
+    <t>INSERT INTO gouser VALUES ('null','2','Adrian Sevillano .','150103','ELMER FAUCETT NRO. 2879 CENTRO AEREO COMERCIAL','13/05/2020 04:14','ana.oliva@talma.com.pe','$2y$10$Z34DID7EwF4QAxkzMDDjm.oeMZd1hYPRfvDMhTwnSNQ0HkH69CMH6','default','19249315','991314155','1','1','Me dedico a la atencion de niños','2');</t>
+  </si>
+  <si>
+    <t>INSERT INTO gouser VALUES ('null','2','Adriana Esmeralda Mansilla Cabezudo','150103','LAS AZUCENAS Nº 1400 URB. LAS BRISAS ','13/05/2020 04:14','isrod2020@hotmail.com','$2y$10$Z34DID7EwF4QAxkzMDDjm.oeMZd1hYPRfvDMhTwnSNQ0HkH69CMH6','default','22312471','992657852','1','1','Me llamo Anthony puente olano , me dedico a la fabricación de paredes , pintado y entre otras cosas','7');</t>
+  </si>
+  <si>
+    <t>INSERT INTO gouser VALUES ('null','2','Adriana Mellado Villa','150103','REPUBLICA DE PANAMA NRO. 5659 DPTO. 304 URB. AURORA ','13/05/2020 04:14','access@asesoriaaccess.com','$2y$10$Z34DID7EwF4QAxkzMDDjm.oeMZd1hYPRfvDMhTwnSNQ0HkH69CMH6','default','15517078','999231845','1','1','Reparo todo tipo de muebles o ventanas , ademas tambien realizo pintado y otras que tenga que ver con el rubro','4');</t>
+  </si>
+  <si>
+    <t>INSERT INTO gouser VALUES ('null','2','Afra Maria  Torres Salas','150103','MRCAL MILLER NRO. 2190 ','13/05/2020 04:14','cshaw@assessmentcenterperu.com','$2y$10$Z34DID7EwF4QAxkzMDDjm.oeMZd1hYPRfvDMhTwnSNQ0HkH69CMH6','default','20960187','995310414','1','1','Reparo impresoras , laptops , escanner , instalación de programas informáticos , Instalación de Redes y cualquier articulo de oficina , espero les guste mi servicio , muchas gracias','7');</t>
+  </si>
+  <si>
+    <t>INSERT INTO gouser VALUES ('null','2','Aguilio Ruiz Rodriguez','150103','ANGAMOS OESTE NRO. 544 DPTO. 302 ','13/05/2020 04:14','intelect@intelect.com.pe','$2y$10$Z34DID7EwF4QAxkzMDDjm.oeMZd1hYPRfvDMhTwnSNQ0HkH69CMH6','default','22007097','992447142','1','1','Me dedico a la atencion de niños','4');</t>
+  </si>
+  <si>
+    <t>INSERT INTO gouser VALUES ('null','2','Agustin Flores Barboza','150103','REPUBLICA DE PANAMA NRO. 4095 ','13/05/2020 04:14','nofloresbarboza@terra.com.pe','$2y$10$Z34DID7EwF4QAxkzMDDjm.oeMZd1hYPRfvDMhTwnSNQ0HkH69CMH6','default','20776368','992625440','1','1','Me llamo Anthony puente olano , me dedico a la fabricación de paredes , pintado y entre otras cosas','7');</t>
+  </si>
+  <si>
+    <t>INSERT INTO gouser VALUES ('null','2','Agustin Gerardo Gamero Nuñez','150103','CARLOS ARRIETA NRO. 1336 URB. SANTA BEATRIZ ','13/05/2020 04:14','agusgame@hotmail.com','$2y$10$Z34DID7EwF4QAxkzMDDjm.oeMZd1hYPRfvDMhTwnSNQ0HkH69CMH6','default','20231381','995945433','1','1','Reparo todo tipo de muebles o ventanas , ademas tambien realizo pintado y otras que tenga que ver con el rubro','5');</t>
+  </si>
+  <si>
+    <t>INSERT INTO gouser VALUES ('null','2','Agustin Sanchez Mallqui','150103','CARABAYA NRO. 500 ','13/05/2020 04:14','aida@veraparedes.org','$2y$10$Z34DID7EwF4QAxkzMDDjm.oeMZd1hYPRfvDMhTwnSNQ0HkH69CMH6','default','12959550','991901126','1','1','Reparo impresoras , laptops , escanner , instalación de programas informáticos , Instalación de Redes y cualquier articulo de oficina , espero les guste mi servicio , muchas gracias','2');</t>
+  </si>
+  <si>
+    <t>INSERT INTO gouser VALUES ('null','2','Aida Dora Vera  Zambrano','150103','LOPEZ DE AYALA NRO. 1298 ','13/05/2020 04:14','aida@veraparedes.org','$2y$10$Z34DID7EwF4QAxkzMDDjm.oeMZd1hYPRfvDMhTwnSNQ0HkH69CMH6','default','12608641','998267761','1','1','Me dedico a la atencion de niños','9');</t>
+  </si>
+  <si>
+    <t>INSERT INTO gouser VALUES ('null','2','Aida Huertas Tacchino','150103','AREQUIPA NRO. 2450 DPTO. 1606 ','13/05/2020 04:14','serviciosjrl@jrlsa.com','$2y$10$Z34DID7EwF4QAxkzMDDjm.oeMZd1hYPRfvDMhTwnSNQ0HkH69CMH6','default','23029092','990579580','1','1','Me llamo Anthony puente olano , me dedico a la fabricación de paredes , pintado y entre otras cosas','5');</t>
+  </si>
+  <si>
+    <t>INSERT INTO gouser VALUES ('null','2','Aida Luz  Zambrano  Valdivia','150103','LOPEZ DE AYALA NRO. 1298 ','13/05/2020 04:14','aida@veraparedes.org','$2y$10$Z34DID7EwF4QAxkzMDDjm.oeMZd1hYPRfvDMhTwnSNQ0HkH69CMH6','default','18167230','991928094','1','1','Reparo todo tipo de muebles o ventanas , ademas tambien realizo pintado y otras que tenga que ver con el rubro','7');</t>
+  </si>
+  <si>
+    <t>INSERT INTO gouser VALUES ('null','2','Aitor Arteta Cilloniz','150103','CADMIO NO.135-129 URB.GRIMANESA','13/05/2020 04:14','gmarina@transberperu.com','$2y$10$Z34DID7EwF4QAxkzMDDjm.oeMZd1hYPRfvDMhTwnSNQ0HkH69CMH6','default','16146069','993873293','1','1','Reparo impresoras , laptops , escanner , instalación de programas informáticos , Instalación de Redes y cualquier articulo de oficina , espero les guste mi servicio , muchas gracias','2');</t>
+  </si>
+  <si>
+    <t>INSERT INTO gouser VALUES ('null','2','Alain Audoyer Uribe','150103',' 41 NRO. 840 ','13/05/2020 04:14','alain_audoyer@coface.com','$2y$10$Z34DID7EwF4QAxkzMDDjm.oeMZd1hYPRfvDMhTwnSNQ0HkH69CMH6','default','20179713','992050596','1','1','Me dedico a la atencion de niños','4');</t>
+  </si>
+  <si>
+    <t>INSERT INTO gouser VALUES ('null','2','Alan  Olaechea Torres','150103','SEPARADORA INDUSTRIAL NRO. 2641 URB. SANTA RAQUEL ','13/05/2020 04:14','mdiezcanseco@bassler.com.pe','$2y$10$Z34DID7EwF4QAxkzMDDjm.oeMZd1hYPRfvDMhTwnSNQ0HkH69CMH6','default','16944885','995530997','1','1','Me llamo Anthony puente olano , me dedico a la fabricación de paredes , pintado y entre otras cosas','1');</t>
+  </si>
+  <si>
+    <t>INSERT INTO gouser VALUES ('null','2','Alan Dell Rodriguez','150103','CORONEL INCLAN NRO. 281 DPTO. 504 ','13/05/2020 04:14','futuros7@hotmail.com','$2y$10$Z34DID7EwF4QAxkzMDDjm.oeMZd1hYPRfvDMhTwnSNQ0HkH69CMH6','default','17487342','991263065','1','1','Reparo todo tipo de muebles o ventanas , ademas tambien realizo pintado y otras que tenga que ver con el rubro','1');</t>
+  </si>
+  <si>
+    <t>INSERT INTO gouser VALUES ('null','2','Alba Lucia Gonzalez  Vargas','150103','LOS EUCALIPTOS Nº 337 DPTO. 402','13/05/2020 04:14','albaluciagonzalez@hotmail.com','$2y$10$Z34DID7EwF4QAxkzMDDjm.oeMZd1hYPRfvDMhTwnSNQ0HkH69CMH6','default','22772081','996510671','1','1','Reparo impresoras , laptops , escanner , instalación de programas informáticos , Instalación de Redes y cualquier articulo de oficina , espero les guste mi servicio , muchas gracias','8');</t>
+  </si>
+  <si>
+    <t>INSERT INTO gouser VALUES ('null','2','Albert Alex Jesus Forsyth  Solari','150103','RIVERA NAVARRETE 501 PISO 19 - EDIFICIO CAPITAL','13/05/2020 04:14','francisco.avendano@eafa.com.pe','$2y$10$Z34DID7EwF4QAxkzMDDjm.oeMZd1hYPRfvDMhTwnSNQ0HkH69CMH6','default','16844276','996476463','1','1','Me dedico a la atencion de niños','4');</t>
+  </si>
+  <si>
+    <t>INSERT INTO gouser VALUES ('null','2','Albert Forsyth Solari','150103','REPUBLICA DE PANAMA NRO. 3411 INT. 13 ','13/05/2020 04:14','anamaria.valdez@forsytharbe.com','$2y$10$Z34DID7EwF4QAxkzMDDjm.oeMZd1hYPRfvDMhTwnSNQ0HkH69CMH6','default','20783688','993846024','1','1','Me llamo Anthony puente olano , me dedico a la fabricación de paredes , pintado y entre otras cosas','2');</t>
   </si>
 </sst>
 </file>
@@ -575,7 +717,17 @@
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -898,8 +1050,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C87F68EA-4E4A-455C-BC03-4D18929A45AC}">
   <dimension ref="A2:AF114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8226,11 +8378,267 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="I3" r:id="rId1" xr:uid="{1AC5571C-39C7-4E1B-B13D-7A4D8F7FFED3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{639F12B8-4656-4DE9-BBC7-9A10C4EE3F83}">
+  <dimension ref="E1:E47"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E47" sqref="E1:E47"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="2" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E2" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="3" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E3" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="4" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E4" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="5" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E5" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="6" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E6" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="7" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E7" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="8" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E8" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="9" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E9" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="10" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E10" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="11" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E11" s="2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="12" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E12" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="13" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E13" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="14" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E14" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="15" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E15" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="16" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E16" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E17" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E18" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="19" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E19" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="20" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E20" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="21" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E21" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="22" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E22" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="23" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E23" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="24" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E24" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="25" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E25" s="2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="26" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E26" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="27" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E27" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="28" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E28" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="29" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E29" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="30" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E30" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="31" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E31" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="32" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E32" s="2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E33" s="2" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="34" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E34" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="35" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E35" s="2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="36" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E36" s="2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="37" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E37" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="38" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E38" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="39" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E39" s="2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="40" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E40" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="41" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E41" s="2" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="42" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E42" s="2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="43" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E43" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="44" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E44" s="2" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="45" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E45" s="2" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="46" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E46" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="47" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E47" t="s">
+        <v>200</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="E1:E47">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>